<commit_message>
Code Changes for RTI Scenario 5 creation
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioSeven201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioSeven201718.xlsx
@@ -1,74 +1,74 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400" firstSheet="47" activeTab="49"/>
+    <workbookView activeTab="49" firstSheet="47" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM1" sheetId="6" r:id="rId3"/>
-    <sheet name="ProcessPayrollForApril" sheetId="7" r:id="rId4"/>
-    <sheet name="ProcessFinalPayrollForApril" sheetId="49" r:id="rId5"/>
-    <sheet name="TestAprilReports" sheetId="11" r:id="rId6"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM2" sheetId="67" r:id="rId7"/>
-    <sheet name="ProcessPayrollForMay" sheetId="68" r:id="rId8"/>
-    <sheet name="ProcessFinalPayrollForMay" sheetId="69" r:id="rId9"/>
-    <sheet name="TestMayReports" sheetId="70" r:id="rId10"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM3" sheetId="71" r:id="rId11"/>
-    <sheet name="ProcessPayrollForJune" sheetId="74" r:id="rId12"/>
-    <sheet name="ProcessFinalPayrollForJune" sheetId="75" r:id="rId13"/>
-    <sheet name="TestJuneReports" sheetId="76" r:id="rId14"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM4" sheetId="77" r:id="rId15"/>
-    <sheet name="ProcessPayrollForJuly" sheetId="78" r:id="rId16"/>
-    <sheet name="ProcessFinalPayrollForJuly" sheetId="79" r:id="rId17"/>
-    <sheet name="TestJulyReports" sheetId="80" r:id="rId18"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM5" sheetId="81" r:id="rId19"/>
-    <sheet name="ProcessPayrollForAug" sheetId="82" r:id="rId20"/>
-    <sheet name="ProcessFinalPayrollForAug" sheetId="83" r:id="rId21"/>
-    <sheet name="TestAugReports" sheetId="84" r:id="rId22"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM6" sheetId="85" r:id="rId23"/>
-    <sheet name="ProcessPayrollForSep" sheetId="86" r:id="rId24"/>
-    <sheet name="ProcessFinalPayrollForSep" sheetId="87" r:id="rId25"/>
-    <sheet name="TestSepReports" sheetId="88" r:id="rId26"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM7" sheetId="89" r:id="rId27"/>
-    <sheet name="ProcessPayrollForOct" sheetId="90" r:id="rId28"/>
-    <sheet name="ProcessFinalPayrollForOct" sheetId="91" r:id="rId29"/>
-    <sheet name="TestOctReports" sheetId="92" r:id="rId30"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM8" sheetId="93" r:id="rId31"/>
-    <sheet name="ProcessPayrollForNov" sheetId="94" r:id="rId32"/>
-    <sheet name="ProcessFinalPayrollForNov" sheetId="95" r:id="rId33"/>
-    <sheet name="TestNovReports" sheetId="96" r:id="rId34"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM9" sheetId="97" r:id="rId35"/>
-    <sheet name="ProcessPayrollForDec" sheetId="98" r:id="rId36"/>
-    <sheet name="ProcessFinalPayrollForDec" sheetId="99" r:id="rId37"/>
-    <sheet name="TestDecReports" sheetId="100" r:id="rId38"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="101" r:id="rId39"/>
-    <sheet name="ProcessPayrollForJan" sheetId="102" r:id="rId40"/>
-    <sheet name="ProcessFinalPayrollForJan" sheetId="103" r:id="rId41"/>
-    <sheet name="TestJanReports" sheetId="104" r:id="rId42"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM11" sheetId="105" r:id="rId43"/>
-    <sheet name="ProcessPayrollForFeb" sheetId="106" r:id="rId44"/>
-    <sheet name="ProcessFinalPayrollForFeb" sheetId="107" r:id="rId45"/>
-    <sheet name="TestFebReports" sheetId="108" r:id="rId46"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM12" sheetId="109" r:id="rId47"/>
-    <sheet name="ProcessPayrollForMarch" sheetId="110" r:id="rId48"/>
-    <sheet name="ProcessFinalPayrollForMarch" sheetId="111" r:id="rId49"/>
-    <sheet name="TestMarchReports" sheetId="112" r:id="rId50"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM1" r:id="rId3" sheetId="6"/>
+    <sheet name="ProcessPayrollForApril" r:id="rId4" sheetId="7"/>
+    <sheet name="ProcessFinalPayrollForApril" r:id="rId5" sheetId="49"/>
+    <sheet name="TestAprilReports" r:id="rId6" sheetId="11"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM2" r:id="rId7" sheetId="67"/>
+    <sheet name="ProcessPayrollForMay" r:id="rId8" sheetId="68"/>
+    <sheet name="ProcessFinalPayrollForMay" r:id="rId9" sheetId="69"/>
+    <sheet name="TestMayReports" r:id="rId10" sheetId="70"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM3" r:id="rId11" sheetId="71"/>
+    <sheet name="ProcessPayrollForJune" r:id="rId12" sheetId="74"/>
+    <sheet name="ProcessFinalPayrollForJune" r:id="rId13" sheetId="75"/>
+    <sheet name="TestJuneReports" r:id="rId14" sheetId="76"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM4" r:id="rId15" sheetId="77"/>
+    <sheet name="ProcessPayrollForJuly" r:id="rId16" sheetId="78"/>
+    <sheet name="ProcessFinalPayrollForJuly" r:id="rId17" sheetId="79"/>
+    <sheet name="TestJulyReports" r:id="rId18" sheetId="80"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM5" r:id="rId19" sheetId="81"/>
+    <sheet name="ProcessPayrollForAug" r:id="rId20" sheetId="82"/>
+    <sheet name="ProcessFinalPayrollForAug" r:id="rId21" sheetId="83"/>
+    <sheet name="TestAugReports" r:id="rId22" sheetId="84"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM6" r:id="rId23" sheetId="85"/>
+    <sheet name="ProcessPayrollForSep" r:id="rId24" sheetId="86"/>
+    <sheet name="ProcessFinalPayrollForSep" r:id="rId25" sheetId="87"/>
+    <sheet name="TestSepReports" r:id="rId26" sheetId="88"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM7" r:id="rId27" sheetId="89"/>
+    <sheet name="ProcessPayrollForOct" r:id="rId28" sheetId="90"/>
+    <sheet name="ProcessFinalPayrollForOct" r:id="rId29" sheetId="91"/>
+    <sheet name="TestOctReports" r:id="rId30" sheetId="92"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM8" r:id="rId31" sheetId="93"/>
+    <sheet name="ProcessPayrollForNov" r:id="rId32" sheetId="94"/>
+    <sheet name="ProcessFinalPayrollForNov" r:id="rId33" sheetId="95"/>
+    <sheet name="TestNovReports" r:id="rId34" sheetId="96"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM9" r:id="rId35" sheetId="97"/>
+    <sheet name="ProcessPayrollForDec" r:id="rId36" sheetId="98"/>
+    <sheet name="ProcessFinalPayrollForDec" r:id="rId37" sheetId="99"/>
+    <sheet name="TestDecReports" r:id="rId38" sheetId="100"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId39" sheetId="101"/>
+    <sheet name="ProcessPayrollForJan" r:id="rId40" sheetId="102"/>
+    <sheet name="ProcessFinalPayrollForJan" r:id="rId41" sheetId="103"/>
+    <sheet name="TestJanReports" r:id="rId42" sheetId="104"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM11" r:id="rId43" sheetId="105"/>
+    <sheet name="ProcessPayrollForFeb" r:id="rId44" sheetId="106"/>
+    <sheet name="ProcessFinalPayrollForFeb" r:id="rId45" sheetId="107"/>
+    <sheet name="TestFebReports" r:id="rId46" sheetId="108"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM12" r:id="rId47" sheetId="109"/>
+    <sheet name="ProcessPayrollForMarch" r:id="rId48" sheetId="110"/>
+    <sheet name="ProcessFinalPayrollForMarch" r:id="rId49" sheetId="111"/>
+    <sheet name="TestMarchReports" r:id="rId50" sheetId="112"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="145">
   <si>
     <t>TC</t>
   </si>
@@ -510,6 +510,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -590,94 +591,94 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="3" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -694,10 +695,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -732,7 +733,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -784,7 +785,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -889,7 +890,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -898,13 +899,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -914,7 +915,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -923,7 +924,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -932,7 +933,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -942,12 +943,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -978,7 +979,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -997,7 +998,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1009,7 +1010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
@@ -1018,10 +1019,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1725,12 +1726,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1739,24 +1740,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="13" max="14" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="45.75" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
@@ -1809,7 +1810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="125.25" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -1854,14 +1855,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1870,15 +1871,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1910,7 +1911,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="94.5" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -1936,12 +1937,12 @@
       <c r="I2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -1950,20 +1951,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2010,7 +2011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="84" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -2052,14 +2053,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2068,20 +2069,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2128,7 +2129,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="78.75" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -2170,14 +2171,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2186,24 +2187,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
@@ -2256,7 +2257,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="115.5" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -2301,14 +2302,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2346,7 +2347,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row ht="135" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -2372,12 +2373,12 @@
       <c r="I2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2386,20 +2387,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2446,7 +2447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="75.75" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -2488,14 +2489,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2504,20 +2505,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2564,7 +2565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="88.5" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -2606,40 +2607,40 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="72" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="72" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="72" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
@@ -2692,7 +2693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="72" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -2743,14 +2744,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2788,7 +2789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row ht="135" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -2814,12 +2815,12 @@
       <c r="I2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2828,10 +2829,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2857,7 +2858,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>51</v>
       </c>
@@ -2875,38 +2876,38 @@
       <c r="G2" s="9"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="57.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="57.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="28.5" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -2950,7 +2951,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="93.75" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -2992,14 +2993,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3008,26 +3009,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -3080,7 +3081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="114.75" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -3127,14 +3128,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3143,24 +3144,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
@@ -3213,7 +3214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="141" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -3258,14 +3259,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3274,15 +3275,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3314,7 +3315,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row ht="135" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -3340,12 +3341,12 @@
       <c r="I2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -3354,20 +3355,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3414,7 +3415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="105" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -3456,14 +3457,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3472,26 +3473,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -3544,7 +3545,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="92.25" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -3591,14 +3592,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -3607,24 +3608,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
@@ -3677,7 +3678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="138.75" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -3722,14 +3723,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3738,15 +3739,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3778,7 +3779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row ht="135" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -3804,12 +3805,12 @@
       <c r="I2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3818,20 +3819,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3878,7 +3879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="133.5" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -3920,42 +3921,42 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="102.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultRowHeight="102.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="61.5" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -4008,7 +4009,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="102.75" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -4055,14 +4056,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4071,10 +4072,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4106,7 +4107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
@@ -4130,13 +4131,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4145,24 +4146,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
@@ -4215,7 +4216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="150" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -4260,14 +4261,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4276,15 +4277,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4316,7 +4317,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row ht="135" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -4342,12 +4343,12 @@
       <c r="I2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -4356,20 +4357,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4416,7 +4417,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="158.25" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -4458,14 +4459,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4474,26 +4475,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -4546,7 +4547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="127.5" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -4593,14 +4594,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4609,24 +4610,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
@@ -4679,7 +4680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="167.25" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -4724,14 +4725,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4740,15 +4741,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4780,7 +4781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row ht="135" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -4806,12 +4807,12 @@
       <c r="I2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -4820,20 +4821,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4880,7 +4881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="103.5" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -4922,14 +4923,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4938,16 +4939,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -5000,7 +5001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="89.25" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -5047,14 +5048,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -5063,24 +5064,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
@@ -5133,7 +5134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="141" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -5178,14 +5179,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5194,15 +5195,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5234,7 +5235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row ht="135" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -5260,12 +5261,12 @@
       <c r="I2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -5274,18 +5275,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5332,7 +5333,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -5372,15 +5373,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5389,19 +5390,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -5445,7 +5446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="93.75" r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -5483,12 +5484,12 @@
       <c r="M2" s="23"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5497,26 +5498,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -5569,7 +5570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="127.5" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -5616,14 +5617,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5632,24 +5633,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
@@ -5702,7 +5703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="150" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -5747,14 +5748,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5763,15 +5764,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -5803,7 +5804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row ht="135" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -5829,12 +5830,12 @@
       <c r="I2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5843,19 +5844,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -5899,7 +5900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="132" r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -5937,12 +5938,12 @@
       <c r="M2" s="23"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5951,26 +5952,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -6023,7 +6024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="132" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -6070,14 +6071,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6086,23 +6087,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
@@ -6155,7 +6156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="140.25" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -6200,14 +6201,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6216,15 +6217,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6256,7 +6257,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row ht="135" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -6282,36 +6283,36 @@
       <c r="I2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="108.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="9.28515625" defaultRowHeight="108.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="34.5" r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
@@ -6352,7 +6353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="143.25" r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
@@ -6390,12 +6391,12 @@
       <c r="M2" s="23"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6404,26 +6405,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -6476,7 +6477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="132" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="132" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -6523,14 +6524,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -6539,18 +6540,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6597,7 +6598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -6637,14 +6638,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -6653,24 +6654,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
@@ -6723,7 +6724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="144.75" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -6768,39 +6769,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="35" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="33.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="1" s="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
@@ -6853,7 +6854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="10" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>32</v>
       </c>
@@ -6902,15 +6903,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6919,15 +6920,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6959,7 +6960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="84" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
@@ -6983,12 +6984,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6997,20 +6998,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7057,7 +7058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -7099,14 +7100,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7115,20 +7116,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7175,7 +7176,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -7217,8 +7218,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
committing files into local system
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioSeven201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioSeven201718.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400" firstSheet="47" activeTab="49"/>
+    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="1" r:id="rId1"/>
@@ -63,12 +63,12 @@
     <sheet name="ProcessFinalPayrollForMarch" sheetId="111" r:id="rId49"/>
     <sheet name="TestMarchReports" sheetId="112" r:id="rId50"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="167">
   <si>
     <t>TC</t>
   </si>
@@ -568,13 +568,16 @@
   </si>
   <si>
     <t>March-2018</t>
+  </si>
+  <si>
+    <t>Week1/Month1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -607,6 +610,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -658,7 +668,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -729,6 +739,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1073,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4061,14 +4074,14 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -4111,8 +4124,8 @@
       <c r="C2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>48</v>
+      <c r="D2" s="28" t="s">
+        <v>166</v>
       </c>
       <c r="E2" s="2">
         <v>470.88</v>
@@ -5248,7 +5261,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6590,7 +6603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>